<commit_message>
working on line partitioning integ tests
</commit_message>
<xml_diff>
--- a/tests/partitioning/traclus_line_partitioning_integration_test_fixture_math.xlsx
+++ b/tests/partitioning/traclus_line_partitioning_integration_test_fixture_math.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>theta</t>
   </si>
@@ -42,10 +42,7 @@
     <t>encoding_cost</t>
   </si>
   <si>
-    <t>total_perp_cost</t>
-  </si>
-  <si>
-    <t>total_angle_cost</t>
+    <t>total perp_cost and angle_cost</t>
   </si>
 </sst>
 </file>
@@ -90,6 +87,206 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.8099518810148729E-2"/>
+          <c:y val="7.4548702245552642E-2"/>
+          <c:w val="0.67149759405074361"/>
+          <c:h val="0.8326195683872849"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>par cost</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$H$3:$H$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$S$3:$S$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>-4.7146366481993205</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.71023663028961925</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.91418642625253055</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9584345865302311</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.736066921261755</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.3614686367055975</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>no par cost</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$3:$I$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.3221478410645684</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.3254467148300728</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.3327220031906153</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.3440140701251453</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.3593863792411707</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.3789269429217872</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="100829440"/>
+        <c:axId val="111150208"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="100829440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="111150208"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="111150208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="100829440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -377,10 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S14"/>
+  <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+      <selection activeCell="D3" sqref="D3:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -406,9 +603,6 @@
       <c r="K2" t="s">
         <v>8</v>
       </c>
-      <c r="M2" t="s">
-        <v>9</v>
-      </c>
       <c r="O2" t="s">
         <v>7</v>
       </c>
@@ -425,34 +619,30 @@
       </c>
       <c r="E3">
         <f>D3 / (2 * COS(RADIANS(H3)))</f>
-        <v>2.5</v>
+        <v>2.5003808201097693</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3">
-        <f>2 * CEILING(LOG(E3, 2), 1)</f>
-        <v>4</v>
+        <f>LOG(2 * E3, 2)</f>
+        <v>2.3221478410645684</v>
       </c>
       <c r="K3">
-        <f>2 * E3 * COS(RADIANS(H3))</f>
-        <v>5</v>
-      </c>
-      <c r="M3">
-        <f>2 * E3 * SIN(RADIANS(H3))</f>
-        <v>0</v>
+        <f>2 * (LOG(2 * E3 * SIN(RADIANS(H3)), 2))</f>
+        <v>-7.0365647430866822</v>
       </c>
       <c r="O3">
-        <f>K3 + M3</f>
-        <v>5</v>
+        <f>K3</f>
+        <v>-7.0365647430866822</v>
       </c>
       <c r="Q3">
-        <f>CEILING(LOG(D3, 2), 1)</f>
-        <v>3</v>
+        <f>LOG(D3, 2)</f>
+        <v>2.3219280948873622</v>
       </c>
       <c r="S3">
         <f>O3+Q3</f>
-        <v>8</v>
+        <v>-4.7146366481993205</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -460,36 +650,32 @@
         <v>5</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E14" si="0">D4 / (2 * COS(RADIANS(H4)))</f>
-        <v>2.5881904510252074</v>
+        <f t="shared" ref="E4:E8" si="0">D4 / (2 * COS(RADIANS(H4)))</f>
+        <v>2.5061047452029306</v>
       </c>
       <c r="H4">
-        <f>H3+15</f>
-        <v>15</v>
+        <f>H3+3</f>
+        <v>4</v>
       </c>
       <c r="I4">
-        <f t="shared" ref="I4:I14" si="1">2 * CEILING(LOG(E4, 2), 1)</f>
-        <v>4</v>
+        <f t="shared" ref="I4:I8" si="1">LOG(2 * E4, 2)</f>
+        <v>2.3254467148300728</v>
       </c>
       <c r="K4">
-        <f t="shared" ref="K4:K14" si="2">2 * E4 * COS(RADIANS(H4))</f>
-        <v>5</v>
-      </c>
-      <c r="M4">
-        <f t="shared" ref="M4:M14" si="3">2 * E4 * SIN(RADIANS(H4))</f>
-        <v>1.3397459621556134</v>
+        <f t="shared" ref="K4:K8" si="2">2 * (LOG(2 * E4 * SIN(RADIANS(H4)), 2))</f>
+        <v>-3.0321647251769814</v>
       </c>
       <c r="O4">
-        <f t="shared" ref="O4:O14" si="4">K4 + M4</f>
-        <v>6.3397459621556136</v>
+        <f t="shared" ref="O4:O20" si="3">K4</f>
+        <v>-3.0321647251769814</v>
       </c>
       <c r="Q4">
-        <f t="shared" ref="Q4:Q14" si="5">CEILING(LOG(D4, 2), 1)</f>
-        <v>3</v>
+        <f t="shared" ref="Q4:Q20" si="4">LOG(D4, 2)</f>
+        <v>2.3219280948873622</v>
       </c>
       <c r="S4">
-        <f t="shared" ref="S4:S14" si="6">O4+Q4</f>
-        <v>9.3397459621556145</v>
+        <f t="shared" ref="S4:S20" si="5">O4+Q4</f>
+        <v>-0.71023663028961925</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -498,35 +684,31 @@
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>2.8867513459481287</v>
+        <v>2.518774563647121</v>
       </c>
       <c r="H5">
-        <f t="shared" ref="H5:H14" si="7">H4+15</f>
-        <v>30</v>
+        <f t="shared" ref="H5:H8" si="6">H4+3</f>
+        <v>7</v>
       </c>
       <c r="I5">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>2.3327220031906153</v>
       </c>
       <c r="K5">
         <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="M5">
-        <f t="shared" si="3"/>
-        <v>2.8867513459481282</v>
+        <v>-1.4077416686348316</v>
       </c>
       <c r="O5">
-        <f t="shared" si="4"/>
-        <v>7.8867513459481282</v>
+        <f t="shared" si="3"/>
+        <v>-1.4077416686348316</v>
       </c>
       <c r="Q5">
-        <f t="shared" si="5"/>
-        <v>3</v>
+        <f t="shared" si="4"/>
+        <v>2.3219280948873622</v>
       </c>
       <c r="S5">
-        <f t="shared" si="6"/>
-        <v>10.886751345948127</v>
+        <f t="shared" si="5"/>
+        <v>0.91418642625253055</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -535,35 +717,31 @@
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>3.5355339059327373</v>
+        <v>2.5385665297143625</v>
       </c>
       <c r="H6">
-        <f t="shared" si="7"/>
-        <v>45</v>
+        <f t="shared" si="6"/>
+        <v>10</v>
       </c>
       <c r="I6">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>2.3440140701251453</v>
       </c>
       <c r="K6">
         <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="M6">
-        <f t="shared" si="3"/>
-        <v>4.9999999999999991</v>
+        <v>-0.36349350835713112</v>
       </c>
       <c r="O6">
-        <f t="shared" si="4"/>
-        <v>10</v>
+        <f t="shared" si="3"/>
+        <v>-0.36349350835713112</v>
       </c>
       <c r="Q6">
-        <f t="shared" si="5"/>
-        <v>3</v>
+        <f t="shared" si="4"/>
+        <v>2.3219280948873622</v>
       </c>
       <c r="S6">
-        <f t="shared" si="6"/>
-        <v>13</v>
+        <f t="shared" si="5"/>
+        <v>1.9584345865302311</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -572,35 +750,31 @@
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>4.9999999999999991</v>
+        <v>2.5657602694834791</v>
       </c>
       <c r="H7">
-        <f t="shared" si="7"/>
-        <v>60</v>
+        <f t="shared" si="6"/>
+        <v>13</v>
       </c>
       <c r="I7">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>2.3593863792411707</v>
       </c>
       <c r="K7">
         <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="M7">
-        <f t="shared" si="3"/>
-        <v>8.6602540378443837</v>
+        <v>0.41413882637439287</v>
       </c>
       <c r="O7">
-        <f t="shared" si="4"/>
-        <v>13.660254037844384</v>
+        <f t="shared" si="3"/>
+        <v>0.41413882637439287</v>
       </c>
       <c r="Q7">
-        <f t="shared" si="5"/>
-        <v>3</v>
+        <f t="shared" si="4"/>
+        <v>2.3219280948873622</v>
       </c>
       <c r="S7">
-        <f t="shared" si="6"/>
-        <v>16.660254037844382</v>
+        <f t="shared" si="5"/>
+        <v>2.736066921261755</v>
       </c>
     </row>
     <row r="8" spans="1:19">
@@ -609,35 +783,31 @@
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>9.6592582628906829</v>
+        <v>2.600748589654005</v>
       </c>
       <c r="H8">
-        <f t="shared" si="7"/>
-        <v>75</v>
+        <f t="shared" si="6"/>
+        <v>16</v>
       </c>
       <c r="I8">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>2.3789269429217872</v>
       </c>
       <c r="K8">
         <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="M8">
-        <f t="shared" si="3"/>
-        <v>18.660254037844386</v>
+        <v>1.0395405418182353</v>
       </c>
       <c r="O8">
-        <f t="shared" si="4"/>
-        <v>23.660254037844386</v>
+        <f t="shared" si="3"/>
+        <v>1.0395405418182353</v>
       </c>
       <c r="Q8">
-        <f t="shared" si="5"/>
-        <v>3</v>
+        <f t="shared" si="4"/>
+        <v>2.3219280948873622</v>
       </c>
       <c r="S8">
-        <f t="shared" si="6"/>
-        <v>26.660254037844386</v>
+        <f t="shared" si="5"/>
+        <v>3.3614686367055975</v>
       </c>
     </row>
     <row r="9" spans="1:19">
@@ -645,35 +815,31 @@
         <v>10</v>
       </c>
       <c r="E9">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E4:E20" si="7">D9 / (2 * COS(RADIANS(H9)))</f>
         <v>5</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="K9">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="M9">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O9">
-        <f t="shared" si="4"/>
-        <v>10</v>
+        <f t="shared" ref="I4:I20" si="8">LOG(2 * E9, 2)</f>
+        <v>3.3219280948873626</v>
+      </c>
+      <c r="K9" t="e">
+        <f t="shared" ref="K4:K20" si="9">2 * (2 * LOG(E9 * SIN(RADIANS(H9)), 2))</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="O9" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
       </c>
       <c r="Q9">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="S9">
-        <f t="shared" si="6"/>
-        <v>14</v>
+        <f t="shared" si="4"/>
+        <v>3.3219280948873626</v>
+      </c>
+      <c r="S9" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="10" spans="1:19">
@@ -681,36 +847,32 @@
         <v>10</v>
       </c>
       <c r="E10">
-        <f t="shared" si="0"/>
-        <v>5.1763809020504148</v>
+        <f t="shared" si="7"/>
+        <v>5.019099187716737</v>
       </c>
       <c r="H10">
-        <f>H9+15</f>
-        <v>15</v>
+        <f>H9 + 5</f>
+        <v>5</v>
       </c>
       <c r="I10">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <f t="shared" si="8"/>
+        <v>3.3274284569986161</v>
       </c>
       <c r="K10">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="M10">
-        <f t="shared" si="3"/>
-        <v>2.6794919243112267</v>
+        <f t="shared" si="9"/>
+        <v>-4.771328020775365</v>
       </c>
       <c r="O10">
-        <f t="shared" si="4"/>
-        <v>12.679491924311227</v>
+        <f t="shared" si="3"/>
+        <v>-4.771328020775365</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="5"/>
-        <v>4</v>
+        <f t="shared" si="4"/>
+        <v>3.3219280948873626</v>
       </c>
       <c r="S10">
-        <f t="shared" si="6"/>
-        <v>16.679491924311229</v>
+        <f t="shared" si="5"/>
+        <v>-1.4493999258880024</v>
       </c>
     </row>
     <row r="11" spans="1:19">
@@ -718,36 +880,32 @@
         <v>10</v>
       </c>
       <c r="E11">
-        <f t="shared" si="0"/>
-        <v>5.7735026918962573</v>
+        <f t="shared" si="7"/>
+        <v>5.0771330594287249</v>
       </c>
       <c r="H11">
-        <f t="shared" si="7"/>
-        <v>30</v>
+        <f t="shared" ref="H11:H14" si="10">H10 + 5</f>
+        <v>10</v>
       </c>
       <c r="I11">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <f t="shared" si="8"/>
+        <v>3.3440140701251448</v>
       </c>
       <c r="K11">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="M11">
-        <f t="shared" si="3"/>
-        <v>5.7735026918962564</v>
+        <f t="shared" si="9"/>
+        <v>-0.72698701671426225</v>
       </c>
       <c r="O11">
-        <f t="shared" si="4"/>
-        <v>15.773502691896256</v>
+        <f t="shared" si="3"/>
+        <v>-0.72698701671426225</v>
       </c>
       <c r="Q11">
-        <f t="shared" si="5"/>
-        <v>4</v>
+        <f t="shared" si="4"/>
+        <v>3.3219280948873626</v>
       </c>
       <c r="S11">
-        <f t="shared" si="6"/>
-        <v>19.773502691896255</v>
+        <f t="shared" si="5"/>
+        <v>2.5949410781731004</v>
       </c>
     </row>
     <row r="12" spans="1:19">
@@ -755,36 +913,32 @@
         <v>10</v>
       </c>
       <c r="E12">
-        <f t="shared" si="0"/>
-        <v>7.0710678118654746</v>
+        <f t="shared" si="7"/>
+        <v>5.1763809020504148</v>
       </c>
       <c r="H12">
-        <f t="shared" si="7"/>
-        <v>45</v>
+        <f t="shared" si="10"/>
+        <v>15</v>
       </c>
       <c r="I12">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <f t="shared" si="8"/>
+        <v>3.3719437814108666</v>
       </c>
       <c r="K12">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="M12">
-        <f t="shared" si="3"/>
-        <v>9.9999999999999982</v>
+        <f t="shared" si="9"/>
+        <v>1.687837871737482</v>
       </c>
       <c r="O12">
-        <f t="shared" si="4"/>
-        <v>20</v>
+        <f t="shared" si="3"/>
+        <v>1.687837871737482</v>
       </c>
       <c r="Q12">
-        <f t="shared" si="5"/>
-        <v>4</v>
+        <f t="shared" si="4"/>
+        <v>3.3219280948873626</v>
       </c>
       <c r="S12">
-        <f t="shared" si="6"/>
-        <v>24</v>
+        <f t="shared" si="5"/>
+        <v>5.0097659666248449</v>
       </c>
     </row>
     <row r="13" spans="1:19">
@@ -792,36 +946,32 @@
         <v>10</v>
       </c>
       <c r="E13">
-        <f t="shared" si="0"/>
-        <v>9.9999999999999982</v>
+        <f t="shared" si="7"/>
+        <v>5.3208888623795607</v>
       </c>
       <c r="H13">
-        <f t="shared" si="7"/>
-        <v>60</v>
+        <f t="shared" si="10"/>
+        <v>20</v>
       </c>
       <c r="I13">
-        <f t="shared" si="1"/>
-        <v>8</v>
+        <f t="shared" si="8"/>
+        <v>3.4116672702060158</v>
       </c>
       <c r="K13">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="M13">
-        <f t="shared" si="3"/>
-        <v>17.320508075688767</v>
+        <f t="shared" si="9"/>
+        <v>3.4552818826580922</v>
       </c>
       <c r="O13">
-        <f t="shared" si="4"/>
-        <v>27.320508075688767</v>
+        <f t="shared" si="3"/>
+        <v>3.4552818826580922</v>
       </c>
       <c r="Q13">
-        <f t="shared" si="5"/>
-        <v>4</v>
+        <f t="shared" si="4"/>
+        <v>3.3219280948873626</v>
       </c>
       <c r="S13">
-        <f t="shared" si="6"/>
-        <v>31.320508075688767</v>
+        <f t="shared" si="5"/>
+        <v>6.7772099775454553</v>
       </c>
     </row>
     <row r="14" spans="1:19">
@@ -829,40 +979,234 @@
         <v>10</v>
       </c>
       <c r="E14">
-        <f t="shared" si="0"/>
-        <v>19.318516525781366</v>
+        <f t="shared" si="7"/>
+        <v>5.5168895948124588</v>
       </c>
       <c r="H14">
+        <f t="shared" si="10"/>
+        <v>25</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="8"/>
+        <v>3.4638551092347685</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="9"/>
+        <v>4.8851284928181551</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="3"/>
+        <v>4.8851284928181551</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="4"/>
+        <v>3.3219280948873626</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="5"/>
+        <v>8.2070565877055177</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
         <f t="shared" si="7"/>
-        <v>75</v>
-      </c>
-      <c r="I14">
-        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="K15" t="e">
+        <f t="shared" si="9"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="O15" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="S15" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="7"/>
+        <v>1.0038198375433474</v>
+      </c>
+      <c r="H16">
+        <f>H15+5</f>
+        <v>5</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="8"/>
+        <v>1.0055003621112535</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="9"/>
+        <v>-14.059040400324816</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="3"/>
+        <v>-14.059040400324816</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="S16">
+        <f t="shared" si="5"/>
+        <v>-13.059040400324816</v>
+      </c>
+    </row>
+    <row r="17" spans="4:19">
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="7"/>
+        <v>1.0154266118857451</v>
+      </c>
+      <c r="H17">
+        <f t="shared" ref="H17:H20" si="11">H16+5</f>
         <v>10</v>
       </c>
-      <c r="K14">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="M14">
-        <f t="shared" si="3"/>
-        <v>37.320508075688771</v>
-      </c>
-      <c r="O14">
-        <f t="shared" si="4"/>
-        <v>47.320508075688771</v>
-      </c>
-      <c r="Q14">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="S14">
-        <f t="shared" si="6"/>
-        <v>51.320508075688771</v>
+      <c r="I17">
+        <f t="shared" si="8"/>
+        <v>1.0220859752377829</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="9"/>
+        <v>-10.014699396263712</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="3"/>
+        <v>-10.014699396263712</v>
+      </c>
+      <c r="Q17">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="S17">
+        <f t="shared" si="5"/>
+        <v>-9.0146993962637119</v>
+      </c>
+    </row>
+    <row r="18" spans="4:19">
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="7"/>
+        <v>1.035276180410083</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="11"/>
+        <v>15</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="8"/>
+        <v>1.050015686523504</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="9"/>
+        <v>-7.5998745078119692</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="3"/>
+        <v>-7.5998745078119692</v>
+      </c>
+      <c r="Q18">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="S18">
+        <f t="shared" si="5"/>
+        <v>-6.5998745078119692</v>
+      </c>
+    </row>
+    <row r="19" spans="4:19">
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="7"/>
+        <v>1.0641777724759121</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="11"/>
+        <v>20</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="8"/>
+        <v>1.0897391753186536</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="9"/>
+        <v>-5.8324304968913578</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="3"/>
+        <v>-5.8324304968913578</v>
+      </c>
+      <c r="Q19">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="S19">
+        <f t="shared" si="5"/>
+        <v>-4.8324304968913578</v>
+      </c>
+    </row>
+    <row r="20" spans="4:19">
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="7"/>
+        <v>1.1033779189624917</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="11"/>
+        <v>25</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="8"/>
+        <v>1.1419270143474063</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="9"/>
+        <v>-4.4025838867312945</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="3"/>
+        <v>-4.4025838867312945</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="S20">
+        <f t="shared" si="5"/>
+        <v>-3.4025838867312945</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>